<commit_message>
holy moly db works boyees
</commit_message>
<xml_diff>
--- a/bin/sampleInventory.xlsx
+++ b/bin/sampleInventory.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>T.V.</t>
+  </si>
+  <si>
+    <t>Cracker</t>
   </si>
 </sst>
 </file>
@@ -442,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,6 +518,23 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <v>100</v>
+      </c>
+      <c r="E5" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed product to include discount price
</commit_message>
<xml_diff>
--- a/bin/sampleInventory.xlsx
+++ b/bin/sampleInventory.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Cracker</t>
+  </si>
+  <si>
+    <t>DiscountPrice</t>
   </si>
 </sst>
 </file>
@@ -445,15 +448,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -464,13 +467,16 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -481,13 +487,16 @@
         <v>2</v>
       </c>
       <c r="D2">
+        <v>1.85</v>
+      </c>
+      <c r="E2">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -498,13 +507,16 @@
         <v>1.5</v>
       </c>
       <c r="D3">
+        <v>1.5</v>
+      </c>
+      <c r="E3">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -515,13 +527,16 @@
         <v>1000</v>
       </c>
       <c r="D4">
+        <v>999</v>
+      </c>
+      <c r="E4">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -532,9 +547,12 @@
         <v>0.5</v>
       </c>
       <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
         <v>100</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>